<commit_message>
Updated samples and extract byte.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,12 +448,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0ca4616a1bbea85344c204b7b099bfb3cdfec68c.bin</t>
+          <t>otxodwlln.exe</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -461,12 +461,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0ebbb4b19aba9667f1715ebb6559b45e8d4c95f8.bin</t>
+          <t>release1.exe</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -474,12 +474,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10c961a86da828a1ba0d2bd6f2e1ce0f2c376d85.bin</t>
+          <t>release10.exe</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -487,12 +487,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>23c8635c484b94e9a18dd5aae8b4146e18a0af3b.bin</t>
+          <t>release11.exe</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -500,12 +500,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2d21bfb45b2eb95e159a1dc4683cf5b34a8156fe.bin</t>
+          <t>release12.exe</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -513,12 +513,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>312fcd79a4a971b2e6ce70dbf07e12bd30716d4b.bin</t>
+          <t>release13.exe</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -526,12 +526,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>31f72418ed907c177ec7acff883186dfcfd4366a.bin</t>
+          <t>release14.exe</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -539,12 +539,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>383f9dd1d965de6dd50f2778073c1274b9715289.bin</t>
+          <t>release15.exe</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -552,12 +552,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3abf98b8f83e66cf55d304949e525d06b3fcb231.bin</t>
+          <t>release2.exe</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -565,12 +565,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4e98fdff10922198a66b0067fc67de5c11757204.bin</t>
+          <t>release3.exe</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -578,12 +578,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4f5af1fc5fd13453c694accd118b82747d60d1a4.bin</t>
+          <t>release31.exe</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -591,12 +591,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4f5cf34996457a9e7b2b3955648c103c8d581a7e.bin</t>
+          <t>release32.exe</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -604,12 +604,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>518857ae1c884b750c16142dbeddc76f2add08c5.bin</t>
+          <t>release33.exe</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -617,12 +617,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>53abeacf36edf47a8c6eb7295e4005533cf93e93.bin</t>
+          <t>release34.exe</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -630,12 +630,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>54056699c0bb803c08e3416fdddabac4d294580c.bin</t>
+          <t>release35.exe</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -643,12 +643,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>543a064f87043586ef8f82041044653cfa7a007d.bin</t>
+          <t>release36.exe</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -656,12 +656,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5d37b60336a37695d7e46a923f98755b9b631537.bin</t>
+          <t>release37.exe</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -669,12 +669,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>629bca7210e11f95f7e396b93c185d90a6abf717.bin</t>
+          <t>release38.exe</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -682,12 +682,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6b0dbbaebeb064a20f3f5415d09d5d2a6913ae51.bin</t>
+          <t>release39.exe</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -695,12 +695,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>6b3bb5aad03a03040040cc44bc9c9a204f1cc63b.bin</t>
+          <t>release40.exe</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -708,12 +708,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6b8650b176fb142366efbd3f4ed18d417fff8060.bin</t>
+          <t>release41.exe</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -721,12 +721,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>6ccd99104f178039d057248c068177f450b17a3a.bin</t>
+          <t>release42.exe</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -734,12 +734,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6ce674531fa3dc1a83b0990679e4842738817544.bin</t>
+          <t>release43.exe</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -747,12 +747,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>7038c938923bee5aa8b435857abe4940a03f5fbb.bin</t>
+          <t>release44.exe</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -760,12 +760,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>721fe735bddf3045cf91da642657731cadacb99f.bin</t>
+          <t>release45.exe</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -773,12 +773,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>72aaafa96b34671fe50be23b2e1a7acb6ea9764d.bin</t>
+          <t>release5.exe</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -786,12 +786,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>86a42c6b8c647d53d206443e0bef8db78cd4ed66.bin</t>
+          <t>release6.exe</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -799,12 +799,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>87dc4dc67787a4c96521afb7109e8271cf4916b1.bin</t>
+          <t>release7.exe</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -812,12 +812,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>90c7dbd713c3b9cf1573fa847730144cb365145f.bin</t>
+          <t>release8.exe</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">{"result":1}
+          <t xml:space="preserve">{"result":0}
 </t>
         </is>
       </c>
@@ -825,309 +825,10 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>989c068f34ff7546e9157d5a8a2f9159a400d147.bin</t>
+          <t>wyyhcszecb.exe</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>a018932c22d17ac8325765acdf62420e9a3c5f85.bin</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>a05c205d38900f583c0aac49bddf275a26f09571.bin</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>a646ed79259a6ae42e4e00211b989b1727914cfc.bin</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>a82155dc4c0041d29ae36b3f31d3489a33ffbefc.bin</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>a887c69811cf126e17a3f4cf0c241daa65365be6.bin</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>b1f41bfc8631a497e62a00301b1dc95d1729cc2d.bin</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>b2ac666de3896462179cd49ca51067a3c80a8bab.bin</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>b7c4bccaa22d03d3710ee4dc6dad7990f5f023af.bin</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>b8ac08c3d1a0741978af89a126ea11fbb15ff24b.bin</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>b9b35a89b499dffb1fddffaed2dd72b71bb14815.bin</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>bdc13b5a66980b23ea4b6ba72f94b52901eb54c0.bin</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>c2558a99f7aef8a2a7daebc28033bbb4459e4131.bin</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>c99fc46d2e47d4d9c1aa58e6d761d862b949d5b0.bin</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>cd709ef8767271ace82f198c33a3ae951c74d3fc.bin</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>da5d33c29a532ec5435147f4fd3a30a8830ff053.bin</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>dc4774d6af984b27662ca4134eda7c6189cb0add.bin</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>ddb0cc4f46bd8624156d47f4b5939c601a822990.bin</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>edd5fe6ebfae61f634196c04ffbb2a75b157215a.bin</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>ee02c72c9d7d36f1dc080a7183f08821a62ab2e5.bin</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>f389e1c970b2ca28112a30a8cfef1f3973fa82ea.bin</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>fd8050db0371f04bc56f91a8f7f6527354e772ab.bin</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>ff6bf03e35cd19902bebbcf50d60884ee3b7e7bd.bin</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{"result":1}
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>ff7ed6920a2adc23f92c063964311796a495a56a.bin</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
         <is>
           <t xml:space="preserve">{"result":1}
 </t>

</xml_diff>